<commit_message>
32 customers, added industrial, commerical and residential data
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/jlhb83_durham_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rando\Desktop\powersystemRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2026" documentId="8_{391B2177-72B6-4110-8D99-6D040AE000E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18A5669F-8A77-41C7-961F-106D31A2F0B7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D2D7A6-3430-42B9-AC4D-7CB76705E9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{863B64AE-D48D-469B-B9B4-5262C76E33AE}"/>
+    <workbookView xWindow="1275" yWindow="3570" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{863B64AE-D48D-469B-B9B4-5262C76E33AE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Reward Func" sheetId="1" r:id="rId1"/>
-    <sheet name="TD3 hyperparmeters" sheetId="2" r:id="rId2"/>
-    <sheet name="Case 3" sheetId="4" r:id="rId3"/>
-    <sheet name="New environment with constraint" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Reward Func" sheetId="1" r:id="rId2"/>
+    <sheet name="TD3 hyperparmeters" sheetId="2" r:id="rId3"/>
+    <sheet name="Case 3" sheetId="4" r:id="rId4"/>
+    <sheet name="New environment with constraint" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="338">
   <si>
     <t>F1</t>
   </si>
@@ -53,12 +54,6 @@
     <t>F4</t>
   </si>
   <si>
-    <t>1) must apply curtailment</t>
-  </si>
-  <si>
-    <t>2) not to set incentive rate to 0</t>
-  </si>
-  <si>
     <t>ones</t>
   </si>
   <si>
@@ -81,9 +76,6 @@
   </si>
   <si>
     <t>w3</t>
-  </si>
-  <si>
-    <t>w4</t>
   </si>
   <si>
     <t>w1</t>
@@ -211,12 +203,6 @@
     <t>warmup</t>
   </si>
   <si>
-    <t>w/ Battery</t>
-  </si>
-  <si>
-    <t>(everything else turned off)</t>
-  </si>
-  <si>
     <t>f1</t>
   </si>
   <si>
@@ -230,12 +216,6 @@
   </si>
   <si>
     <t>charging</t>
-  </si>
-  <si>
-    <t>discharging</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>4(DDPG)</t>
@@ -372,9 +352,6 @@
   </si>
   <si>
     <t>actually MGO_profit is around 260</t>
-  </si>
-  <si>
-    <t>curr best</t>
   </si>
   <si>
     <t>N/A</t>
@@ -1135,18 +1112,6 @@
   </si>
   <si>
     <t>next step constrain SOC without constraining pbat</t>
-  </si>
-  <si>
-    <t>PSO</t>
-  </si>
-  <si>
-    <t>PSO reocnfig</t>
-  </si>
-  <si>
-    <t>DDPG reconfig</t>
-  </si>
-  <si>
-    <t>action</t>
   </si>
 </sst>
 </file>
@@ -2196,84 +2161,296 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5E91F6-23D2-4569-A29F-B220EDAE36EC}">
-  <dimension ref="B1:R32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724D1E31-25BF-4676-AE02-AE5B326C23CB}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="7">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5E91F6-23D2-4569-A29F-B220EDAE36EC}">
+  <dimension ref="B1:Q20"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="s">
-        <v>348</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>346</v>
-      </c>
-      <c r="R2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -2301,25 +2478,16 @@
       <c r="J3" s="1">
         <v>4500</v>
       </c>
-      <c r="K3" s="1">
-        <v>4952.4295000000002</v>
+      <c r="K3" s="2">
+        <v>3855</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="1">
-        <v>4406.29</v>
-      </c>
-      <c r="P3" s="4">
-        <v>4393.3599999999997</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>4432.3</v>
-      </c>
-      <c r="R3">
-        <v>4429.5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O3" s="1"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2347,24 +2515,15 @@
       <c r="J4">
         <v>640.94000000000005</v>
       </c>
-      <c r="K4">
-        <v>725.26909999999998</v>
+      <c r="K4" s="3">
+        <v>574</v>
       </c>
       <c r="N4" s="1"/>
-      <c r="O4" s="1">
-        <v>624.75</v>
-      </c>
-      <c r="P4" s="4">
-        <v>650.20000000000005</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>594.74</v>
-      </c>
-      <c r="R4">
-        <v>521.77</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O4" s="1"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2392,24 +2551,15 @@
       <c r="J5">
         <v>298.92</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>0</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="1">
-        <v>368.43</v>
-      </c>
-      <c r="P5" s="4">
-        <v>370.74</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>374.61</v>
-      </c>
-      <c r="R5">
-        <v>374.4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O5" s="1"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -2437,314 +2587,95 @@
       <c r="J6" s="1">
         <v>-30</v>
       </c>
-      <c r="K6" s="1">
-        <v>218.5874</v>
+      <c r="K6" s="2">
+        <v>0</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="O6" s="1"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ref="C7:K7" si="0">-$C$18*C3-$C$19*C4+$C$20*C5-$C$21*C6</f>
-        <v>-747826.57038461545</v>
+        <v>-145.45124999999999</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>27409.815384615387</v>
+        <v>-306.0333333333333</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>-430.30769230769238</v>
+        <v>-466.16666666666663</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>-769248.4769230769</v>
+        <v>-19.18333333333328</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>-221.31081538461544</v>
+        <v>-242.25338333333335</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>-430.30769230769238</v>
+        <v>-466.16666666666663</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>-76824.573076923072</v>
+        <v>106.71250000000009</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="0"/>
-        <v>-163.21076923076922</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="0"/>
-        <v>-453.5604615384616</v>
+        <v>-179.31166666666667</v>
+      </c>
+      <c r="K7" s="2">
+        <f>-$C$18*K3-$C$19*K4+$C$20*K5-K6</f>
+        <v>-369.08333333333331</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7">
-        <f>-$C$18*O3-$C$19*O4+$C$20*O5-$C$21*O6</f>
-        <v>-103.5953846153846</v>
-      </c>
-      <c r="P7">
-        <f>-$C$18*P3-$C$19*P4+$C$20*P5-$C$21*P6</f>
-        <v>-102.78153846153839</v>
-      </c>
-      <c r="Q7">
-        <f>-$C$18*Q3-$C$19*Q4+$C$20*Q5-$C$21*Q6</f>
-        <v>-98.533846153846184</v>
-      </c>
-      <c r="R7">
-        <f>-$C$18*R3-$C$19*R4+$C$20*R5-$C$21*R6</f>
-        <v>-92.866923076923058</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="M14" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="L16" t="s">
-        <v>57</v>
-      </c>
-      <c r="M16">
-        <v>0.19231306117024299</v>
-      </c>
-      <c r="N16">
-        <v>0.21017240677316801</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="L17" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17">
-        <v>1.93459588946065E-2</v>
-      </c>
-      <c r="N17">
-        <v>2.0759499302171799E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <f>D18/($D$18+$D$19+$D$20+$D$21)</f>
-        <v>7.6923076923076927E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="L18" t="s">
-        <v>59</v>
-      </c>
-      <c r="M18">
-        <v>0.339065974663815</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:C21" si="1">D19/($D$18+$D$19+$D$20+$D$21)</f>
-        <v>7.6923076923076927E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="L19" t="s">
-        <v>60</v>
-      </c>
-      <c r="M19">
-        <v>8.5899562507950097E-2</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>0.76923076923076927</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D20">
         <v>10</v>
-      </c>
-      <c r="L20" t="s">
-        <v>273</v>
-      </c>
-      <c r="M20">
-        <v>-1.8010984191372299</v>
-      </c>
-      <c r="N20">
-        <v>-1.9443892426781599</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="G22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23">
-        <v>6017.4295000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24">
-        <v>891.11199999999997</v>
-      </c>
-      <c r="L24" t="s">
-        <v>57</v>
-      </c>
-      <c r="M24">
-        <f>M16+M17</f>
-        <v>0.21165902006484949</v>
-      </c>
-      <c r="N24">
-        <f>N16+N17</f>
-        <v>0.23093190607533981</v>
-      </c>
-      <c r="O24">
-        <f>M24/N24</f>
-        <v>0.91654299166351361</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>58</v>
-      </c>
-      <c r="M25">
-        <v>0.339065974663815</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26">
-        <v>350541.4743</v>
-      </c>
-      <c r="L26" t="s">
-        <v>59</v>
-      </c>
-      <c r="M26">
-        <v>-1.8010984191372299</v>
-      </c>
-      <c r="N26">
-        <v>-1.9443892426781599</v>
-      </c>
-      <c r="O26">
-        <f>M26/N26</f>
-        <v>0.92630548431569992</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29">
-        <v>3887.4295000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F30" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30">
-        <v>626.18219999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F31" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="I31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F32" t="s">
-        <v>60</v>
-      </c>
-      <c r="G32">
-        <v>613804.08160000003</v>
       </c>
     </row>
   </sheetData>
@@ -2753,167 +2684,167 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059023FD-5C0F-4576-A068-016E2D5484D1}">
   <dimension ref="B1:AA41"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="B2:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4"/>
-    <col min="2" max="2" width="26.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="4"/>
-    <col min="4" max="4" width="12.88671875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="26.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="12.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="23" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" customWidth="1"/>
-    <col min="7" max="10" width="9.109375" style="4"/>
+    <col min="6" max="6" width="15.7109375" style="4" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" style="4"/>
     <col min="11" max="11" width="11" style="4" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" style="4" customWidth="1"/>
-    <col min="13" max="17" width="12.6640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="27.5546875" style="4" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="12.88671875" style="4" customWidth="1"/>
-    <col min="21" max="21" width="29.33203125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="12.5546875" style="4" customWidth="1"/>
-    <col min="23" max="23" width="12.88671875" style="4" customWidth="1"/>
-    <col min="24" max="26" width="9.109375" style="4"/>
-    <col min="27" max="27" width="19.6640625" style="4" customWidth="1"/>
-    <col min="28" max="16384" width="9.109375" style="4"/>
+    <col min="12" max="12" width="14.85546875" style="4" customWidth="1"/>
+    <col min="13" max="17" width="12.7109375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="27.5703125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" style="4" customWidth="1"/>
+    <col min="21" max="21" width="29.28515625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" style="4" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" style="4" customWidth="1"/>
+    <col min="24" max="26" width="9.140625" style="4"/>
+    <col min="27" max="27" width="19.7109375" style="4" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
       <c r="R1" s="4" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="P3" s="4">
         <v>8</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="U3" s="4">
         <v>13</v>
@@ -2934,12 +2865,12 @@
         <v>18</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="7">
         <v>1E-3</v>
@@ -3005,9 +2936,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4">
         <v>0.6</v>
@@ -3064,7 +2995,7 @@
         <v>0.3</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="Y5" s="4">
         <v>2</v>
@@ -3073,9 +3004,9 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -3099,7 +3030,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="M6" s="4">
         <v>0</v>
@@ -3132,60 +3063,60 @@
         <v>0</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="AA6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K7" s="4">
         <v>0.3</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="S7" s="4">
         <v>0.3</v>
@@ -3197,21 +3128,21 @@
         <v>0.3</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AA7" s="8">
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4">
         <v>1.4999999999999999E-4</v>
@@ -3235,7 +3166,7 @@
         <v>1E-4</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M8" s="4">
         <v>1E-4</v>
@@ -3268,154 +3199,154 @@
         <v>1E-4</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AA8" s="8">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L9" s="4">
         <v>256</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="Y9" s="4">
         <v>256</v>
       </c>
       <c r="AA9" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L10" s="4">
         <v>0.9</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="Y10" s="4">
         <v>0.9</v>
       </c>
       <c r="AA10" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4">
         <v>256</v>
@@ -3481,9 +3412,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E12" s="4">
         <v>0.9</v>
@@ -3549,9 +3480,9 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4">
         <v>64</v>
@@ -3617,9 +3548,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -3685,63 +3616,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L15" s="4">
         <v>2500</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="W15" s="4">
         <v>2500</v>
@@ -3750,12 +3681,12 @@
         <v>2500</v>
       </c>
       <c r="AA15" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E16" s="7">
         <v>20000</v>
@@ -3821,83 +3752,83 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="17" spans="2:27" s="6" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:27" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="K17" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="M17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="N17" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="O17" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="Q17" s="10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="T17" s="10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="V17" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="W17" s="6" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="X17" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="Y17" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="Z17" s="6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="AA17" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F18" s="4">
         <v>-135</v>
@@ -3921,13 +3852,13 @@
         <v>-161</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="N18" s="4">
         <v>-39.9238</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="P18" s="4">
         <v>-427</v>
@@ -3948,18 +3879,18 @@
         <v>-126</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="AA18" s="4">
         <v>-170</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G19" s="7">
         <v>4497.6531000000004</v>
@@ -4007,18 +3938,18 @@
         <v>4405.0510000000004</v>
       </c>
       <c r="Z19" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="AA19" s="4">
         <v>4468</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G20" s="7">
         <v>666.12390000000005</v>
@@ -4066,18 +3997,18 @@
         <v>651.23990000000003</v>
       </c>
       <c r="Z20" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="AA20" s="4">
         <v>634</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G21" s="4">
         <v>311.75</v>
@@ -4125,18 +4056,18 @@
         <v>368.86349999999999</v>
       </c>
       <c r="Z21" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="AA21" s="4">
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G22" s="4">
         <v>-1256.3349000000001</v>
@@ -4184,15 +4115,15 @@
         <v>276.47910000000002</v>
       </c>
       <c r="Z22" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="AA22" s="4">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G23" s="4">
         <v>-101</v>
@@ -4207,7 +4138,7 @@
         <v>-76</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="P23" s="4">
         <v>-296</v>
@@ -4231,55 +4162,55 @@
         <v>-68</v>
       </c>
       <c r="Z23" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="AA23" s="4">
         <v>-45</v>
       </c>
     </row>
-    <row r="24" spans="2:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:27" ht="195" x14ac:dyDescent="0.25">
       <c r="L24" s="11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="S24" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="W24" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="T24" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="W24" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="T28" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5">
@@ -4304,9 +4235,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5">
@@ -4331,9 +4262,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5">
@@ -4358,9 +4289,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5">
@@ -4382,9 +4313,9 @@
         <v>0.72018348623853212</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5">
@@ -4406,7 +4337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -4415,7 +4346,7 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -4424,14 +4355,14 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="S35" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="T35" s="4">
         <f t="shared" ref="T35:T36" si="2">T28*T19/13</f>
         <v>337.95048461538465</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -4440,16 +4371,16 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="S36" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="T36" s="4">
         <f t="shared" si="2"/>
         <v>50.019223076923076</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="12">
@@ -4471,16 +4402,16 @@
         <v>1.0169901312124399</v>
       </c>
       <c r="S37" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="T37" s="4">
         <f>T30*T21/13</f>
         <v>285.18623076923075</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5">
@@ -4502,16 +4433,16 @@
         <v>0.97500976163164343</v>
       </c>
       <c r="S38" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="T38" s="4">
         <f>T31*T22/13</f>
         <v>13.614415384615386</v>
       </c>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5">
@@ -4533,9 +4464,9 @@
         <v>0.81188513524630734</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5">
@@ -4557,9 +4488,9 @@
         <v>0.9458976086550871</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5">
@@ -4591,37 +4522,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA069BE6-C338-4F55-ACE4-D9DF040301EB}">
   <dimension ref="C3:S103"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="5" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="5" customWidth="1"/>
     <col min="10" max="10" width="11" style="5" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="21.109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="5" customWidth="1"/>
     <col min="15" max="17" width="9" style="5"/>
     <col min="18" max="18" width="13" style="5" customWidth="1"/>
     <col min="19" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -4663,47 +4594,47 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" s="12">
         <v>1E-3</v>
@@ -4736,9 +4667,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5">
         <v>0.5</v>
@@ -4768,9 +4699,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -4800,41 +4731,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5">
         <v>1.4999999999999999E-4</v>
@@ -4864,73 +4795,73 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5">
         <v>256</v>
@@ -4939,10 +4870,10 @@
         <v>256</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="K12" s="4">
         <v>256</v>
@@ -4966,9 +4897,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5">
         <v>0.9</v>
@@ -4998,9 +4929,9 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E14" s="5">
         <v>128</v>
@@ -5030,9 +4961,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" s="5">
         <v>2</v>
@@ -5062,41 +4993,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E17" s="12">
         <v>20000</v>
@@ -5126,53 +5057,53 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="18" spans="3:19" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:19" ht="180" x14ac:dyDescent="0.25">
       <c r="C18" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="H18" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="I18" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>149</v>
-      </c>
       <c r="K18" s="15" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="M18" s="15" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="P18" s="15" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="R18" s="15" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E19" s="12">
         <v>-8939000</v>
@@ -5187,13 +5118,13 @@
         <v>-5.8579999999999997</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="O19" s="5">
         <v>-2.1734</v>
       </c>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
         <v>0</v>
       </c>
@@ -5207,16 +5138,16 @@
         <v>4766.2375000000002</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
         <v>1</v>
       </c>
@@ -5230,16 +5161,16 @@
         <v>671.03909999999996</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
@@ -5253,16 +5184,16 @@
         <v>83.475300000000004</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="5" t="s">
         <v>3</v>
       </c>
@@ -5276,18 +5207,18 @@
         <v>7197.5775999999996</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E24" s="12"/>
       <c r="G24" s="5">
@@ -5297,76 +5228,76 @@
         <v>-64.4071</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="3:19" ht="72" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="3:19" ht="75" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="M26" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E31" s="17"/>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C32" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="5">
         <v>-2.6371000000000002</v>
       </c>
@@ -5392,332 +5323,332 @@
         <v>-2.0024999999999999</v>
       </c>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D39" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D40" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D46" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D49" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D39" s="5" t="s">
+      <c r="D51" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C52" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D40" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D41" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D42" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D43" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D44" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D45" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="K45" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D46" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D47" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D48" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="K48" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D49" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="K49" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C51" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C52" s="5" t="s">
-        <v>272</v>
       </c>
       <c r="D52" s="5">
         <v>-2.5703</v>
@@ -5726,9 +5657,9 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C54" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D54" s="5">
         <v>1.1100000000000001</v>
@@ -5737,9 +5668,9 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C55" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D55" s="5">
         <v>1.1385000000000001</v>
@@ -5748,25 +5679,25 @@
         <v>1.069</v>
       </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C56" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D56" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C57" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D57" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C58" s="5" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D58" s="5">
         <v>-57.116700000000002</v>
@@ -5775,37 +5706,37 @@
         <v>-50.149000000000001</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E62" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C64" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="65" spans="4:8" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D65" s="5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="66" spans="4:8" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D66" s="5">
         <v>-2.1413000000000002</v>
       </c>
@@ -5822,236 +5753,236 @@
         <v>-1.8320000000000001</v>
       </c>
     </row>
-    <row r="68" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="69" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D69" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="E68" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="F68" s="5" t="s">
+      <c r="F69" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="H69" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D70" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D71" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D72" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="73" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D73" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="74" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D74" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="75" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D75" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="76" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D76" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="77" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D77" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="78" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D78" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D79" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="80" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D80" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D88" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H68" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="69" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D69" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="70" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D70" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="71" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D71" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="72" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D72" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="73" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D73" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="74" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D74" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="75" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D75" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="76" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D76" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="77" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D77" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="78" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D78" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="79" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D79" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="80" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D80" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D88" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="F88" s="5" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="89" spans="4:8" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D89" s="5">
         <v>-2.4992999999999999</v>
       </c>
@@ -6068,213 +5999,213 @@
         <v>-1.9625999999999999</v>
       </c>
     </row>
-    <row r="91" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D91" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D92" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="92" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D92" s="5" t="s">
+      <c r="F92" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="93" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D93" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="94" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D94" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D95" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="F95" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="G95" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="G92" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="93" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D93" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G93" s="5" t="s">
+      <c r="H95" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="96" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D96" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D97" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="98" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D98" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="99" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D99" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="100" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D100" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="101" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D101" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D102" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="103" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D94" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G94" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D95" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D96" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="97" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D97" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="98" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D98" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="99" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D99" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="G99" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="H99" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="100" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D100" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G100" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H100" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="101" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D101" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G101" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H101" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="102" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D102" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="G102" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="H102" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="103" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="H103" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -6284,23 +6215,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F9E9A0-4B76-457B-8E88-3A993889FFC4}">
   <dimension ref="B2:N93"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="T78" sqref="T78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D2" s="4">
         <v>11</v>
       </c>
@@ -6308,20 +6239,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4">
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="12">
         <v>1E-4</v>
@@ -6333,9 +6264,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="7">
         <v>0.2</v>
@@ -6347,9 +6278,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
@@ -6361,23 +6292,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" s="7">
         <v>4.0000000000000002E-4</v>
@@ -6389,37 +6320,37 @@
         <v>9.0000000000000006E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5">
         <v>512</v>
@@ -6431,9 +6362,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4">
         <v>0.9</v>
@@ -6445,9 +6376,9 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4">
         <v>128</v>
@@ -6459,9 +6390,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="4">
         <v>2</v>
@@ -6473,9 +6404,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -6487,9 +6418,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="7">
         <v>1500</v>
@@ -6501,29 +6432,29 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="195" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="4">
         <v>-256</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
@@ -6531,7 +6462,7 @@
         <v>4670.9998999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
@@ -6539,7 +6470,7 @@
         <v>688.9171</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
@@ -6547,7 +6478,7 @@
         <v>16.5168</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
@@ -6555,36 +6486,36 @@
         <v>-3340.0697</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E46" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J46" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="N46" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -6594,23 +6525,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a5f30f06-3ff7-49e3-bc32-23ae53d395df" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F29E890B1677942AC5CC5B4ACED935E" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7da710de07744ec43c376f64a408a3f1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a5f30f06-3ff7-49e3-bc32-23ae53d395df" xmlns:ns4="b0358a3f-35e9-43e8-92b1-81a7ee99952e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fa12d63991276b0105eaadee37a51aa" ns3:_="" ns4:_="">
     <xsd:import namespace="a5f30f06-3ff7-49e3-bc32-23ae53d395df"/>
@@ -6857,32 +6771,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10687E7C-85AB-48B6-BA13-9095F4C72800}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b0358a3f-35e9-43e8-92b1-81a7ee99952e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a5f30f06-3ff7-49e3-bc32-23ae53d395df"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2285E236-9903-4E23-B4DD-9367E35E4AD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a5f30f06-3ff7-49e3-bc32-23ae53d395df" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF22150D-C9A8-4C06-9A4B-F95F0DA92B48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6899,4 +6805,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2285E236-9903-4E23-B4DD-9367E35E4AD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10687E7C-85AB-48B6-BA13-9095F4C72800}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b0358a3f-35e9-43e8-92b1-81a7ee99952e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a5f30f06-3ff7-49e3-bc32-23ae53d395df"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed reconfiguration (double check how generator power should be calculated
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rando\Desktop\powersystemRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9F1433-6342-4AA1-A1B1-39D298CB71D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558E09CF-2616-4488-B6CC-01BAB23D54CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{863B64AE-D48D-469B-B9B4-5262C76E33AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{863B64AE-D48D-469B-B9B4-5262C76E33AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="343">
   <si>
     <t>F1</t>
   </si>
@@ -1115,6 +1115,18 @@
   </si>
   <si>
     <t>grad threshold</t>
+  </si>
+  <si>
+    <t>DDPG agent</t>
+  </si>
+  <si>
+    <t>reconfig</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>didn’t work</t>
   </si>
 </sst>
 </file>
@@ -2165,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724D1E31-25BF-4676-AE02-AE5B326C23CB}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,15 +2189,21 @@
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -2194,8 +2212,11 @@
       <c r="D2" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -2204,8 +2225,14 @@
       <c r="D3" s="7">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -2214,8 +2241,14 @@
       <c r="D4" s="4">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0.6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>338</v>
       </c>
@@ -2224,8 +2257,14 @@
       <c r="D5" s="4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>93</v>
       </c>
@@ -2234,8 +2273,14 @@
       <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -2244,8 +2289,14 @@
       <c r="D7" s="7">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -2254,8 +2305,14 @@
       <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -2264,8 +2321,14 @@
       <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -2274,8 +2337,14 @@
       <c r="D10" s="4">
         <v>512</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="4">
+        <v>512</v>
+      </c>
+      <c r="F10" s="4">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -2284,8 +2353,14 @@
       <c r="D11" s="4">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -2294,8 +2369,14 @@
       <c r="D12" s="4">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="4">
+        <v>64</v>
+      </c>
+      <c r="F12" s="4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -2304,8 +2385,14 @@
       <c r="D13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
@@ -2314,8 +2401,14 @@
       <c r="D14" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
@@ -2324,62 +2417,97 @@
       <c r="D15" s="7">
         <v>15000</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="E15" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F15" s="7">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>341</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>0</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="4">
+        <v>227.72044</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="4">
+        <v>2957.8833</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="4">
+        <v>508.47464000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="4">
+        <v>626.06859999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>342</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2691,8 +2819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059023FD-5C0F-4576-A068-016E2D5484D1}">
   <dimension ref="B1:AA41"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,7 +2831,8 @@
     <col min="4" max="4" width="12.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="23" style="4" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="4" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="4"/>
+    <col min="7" max="7" width="16.140625" style="4" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="4"/>
     <col min="11" max="11" width="11" style="4" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" style="4" customWidth="1"/>
     <col min="13" max="17" width="12.7109375" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
added case II training, finalised hyperparameters
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rando\Desktop\powersystemRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFF9E18-B21A-423F-BB8C-7F4E750B58C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB645C45-C6BD-4EAC-A796-E160D641B0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{863B64AE-D48D-469B-B9B4-5262C76E33AE}"/>
+    <workbookView xWindow="-23148" yWindow="-72" windowWidth="23256" windowHeight="12456" xr2:uid="{863B64AE-D48D-469B-B9B4-5262C76E33AE}"/>
   </bookViews>
   <sheets>
     <sheet name="REVISION" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="360">
   <si>
     <t>F1</t>
   </si>
@@ -1176,6 +1176,12 @@
   </si>
   <si>
     <t>1024 512</t>
+  </si>
+  <si>
+    <t>216 512</t>
+  </si>
+  <si>
+    <t>EXPLORATION DIDN’T SET PORPERLY</t>
   </si>
 </sst>
 </file>
@@ -1303,8 +1309,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2229,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724D1E31-25BF-4676-AE02-AE5B326C23CB}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2247,7 @@
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2257,8 +2263,14 @@
       <c r="G1" s="4" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -2272,7 +2284,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>350</v>
       </c>
@@ -2293,8 +2305,11 @@
       <c r="H3" s="7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>349</v>
       </c>
@@ -2315,8 +2330,11 @@
       <c r="H4" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="13">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>338</v>
       </c>
@@ -2337,8 +2355,11 @@
       <c r="H5">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I5" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>347</v>
       </c>
@@ -2353,14 +2374,17 @@
       <c r="F6" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="4" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="19">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -2381,8 +2405,11 @@
       <c r="H7" s="7">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="7">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -2403,8 +2430,11 @@
       <c r="H8" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -2425,8 +2455,11 @@
       <c r="H9" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -2447,8 +2480,11 @@
       <c r="H10" s="4" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -2469,8 +2505,11 @@
       <c r="H11" s="4">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -2491,8 +2530,11 @@
       <c r="H12" s="4">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -2513,8 +2555,11 @@
       <c r="H13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>354</v>
       </c>
@@ -2529,8 +2574,11 @@
       <c r="H14" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>346</v>
       </c>
@@ -2547,8 +2595,11 @@
       <c r="H15" s="4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>343</v>
       </c>
@@ -2569,8 +2620,11 @@
       <c r="H16" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -2591,8 +2645,11 @@
       <c r="H17" s="1">
         <v>10000</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>340</v>
       </c>
@@ -2613,8 +2670,11 @@
       <c r="H18" s="7" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="I18" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
@@ -2634,7 +2694,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
@@ -2647,7 +2707,7 @@
         <v>-34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
@@ -2665,8 +2725,11 @@
       <c r="G21" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>1</v>
       </c>
@@ -2682,7 +2745,7 @@
         <v>526.16088999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>2</v>
       </c>
@@ -2698,7 +2761,7 @@
         <v>85.508101999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>3</v>
       </c>
@@ -2712,7 +2775,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>60</v>
       </c>
@@ -6568,7 +6631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F9E9A0-4B76-457B-8E88-3A993889FFC4}">
   <dimension ref="B2:N93"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="T78" sqref="T78"/>
     </sheetView>
   </sheetViews>
@@ -6874,12 +6937,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a5f30f06-3ff7-49e3-bc32-23ae53d395df" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7130,17 +7192,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a5f30f06-3ff7-49e3-bc32-23ae53d395df" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2285E236-9903-4E23-B4DD-9367E35E4AD3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10687E7C-85AB-48B6-BA13-9095F4C72800}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b0358a3f-35e9-43e8-92b1-81a7ee99952e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a5f30f06-3ff7-49e3-bc32-23ae53d395df"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7165,18 +7237,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10687E7C-85AB-48B6-BA13-9095F4C72800}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2285E236-9903-4E23-B4DD-9367E35E4AD3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b0358a3f-35e9-43e8-92b1-81a7ee99952e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a5f30f06-3ff7-49e3-bc32-23ae53d395df"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>